<commit_message>
Added lots of build systems
</commit_message>
<xml_diff>
--- a/build-systems-table.xlsx
+++ b/build-systems-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cartermelnick/research/build-systems-shootout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62BBE032-1AD9-7048-9471-D66E966D3716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC17B25-DE10-D944-AF0B-9AE04FADAD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{AB1A8EDA-4843-BD4E-AEE0-5FA5614A28B5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="130">
   <si>
     <t>Build System</t>
   </si>
@@ -72,15 +72,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Seemingly?</t>
-  </si>
-  <si>
     <t>Not always</t>
   </si>
   <si>
-    <t>Uncertain if antidependencies are handled</t>
-  </si>
-  <si>
     <t>Partial support - you have to run Fac multiple times if you don't specify</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Unsure</t>
   </si>
   <si>
-    <t>Seemingly. Though I haven't found an implementation to test</t>
-  </si>
-  <si>
     <t>https://ifl21.cs.ru.nl/Program?action=download&amp;upname=IFL21_Mokhov.pdf</t>
   </si>
   <si>
@@ -186,13 +177,253 @@
     <t>https://redo.readthedocs.io/en/latest/</t>
   </si>
   <si>
-    <t>Nix</t>
-  </si>
-  <si>
-    <t>https://edolstra.github.io/pubs/nspfssd-lisa2004-final.pdf</t>
-  </si>
-  <si>
-    <t>Not a build system - a deploy system</t>
+    <t>Tested?</t>
+  </si>
+  <si>
+    <t>No - directories are not handled properly every time</t>
+  </si>
+  <si>
+    <t>Does not support anti-dependencies</t>
+  </si>
+  <si>
+    <t>No - successfully installed and set up the tool, but ran into an issue with fsatrace when attempting to build a project</t>
+  </si>
+  <si>
+    <t>No - I don't know OCaml</t>
+  </si>
+  <si>
+    <t>No - couldn't figure out how to set up</t>
+  </si>
+  <si>
+    <t>No - installation failure</t>
+  </si>
+  <si>
+    <t>No - installation didn't seem to work</t>
+  </si>
+  <si>
+    <t>Amake</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/pdf/10.5555/2663360.2663361</t>
+  </si>
+  <si>
+    <t>A modified version of Make that allows for automatic dependency detection</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>https://docs.haskellstack.org/en/stable/README/</t>
+  </si>
+  <si>
+    <t>Cabal</t>
+  </si>
+  <si>
+    <t>https://www.haskell.org/cabal/</t>
+  </si>
+  <si>
+    <t>Buildr</t>
+  </si>
+  <si>
+    <t>https://buildr.apache.org/</t>
+  </si>
+  <si>
+    <t>Grunt</t>
+  </si>
+  <si>
+    <t>https://gruntjs.com/</t>
+  </si>
+  <si>
+    <t>Rake</t>
+  </si>
+  <si>
+    <t>https://github.com/ruby/rake</t>
+  </si>
+  <si>
+    <t>A-A-P</t>
+  </si>
+  <si>
+    <t>http://www.a-a-p.org/</t>
+  </si>
+  <si>
+    <t>Buildout</t>
+  </si>
+  <si>
+    <t>http://www.buildout.org/en/latest/</t>
+  </si>
+  <si>
+    <t>Gradle</t>
+  </si>
+  <si>
+    <t>https://gradle.org/</t>
+  </si>
+  <si>
+    <t>Gulp</t>
+  </si>
+  <si>
+    <t>https://gulpjs.com/</t>
+  </si>
+  <si>
+    <t>ASDF</t>
+  </si>
+  <si>
+    <t>https://asdf.common-lisp.dev/</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
+  <si>
+    <t>https://www.boost.org/build/</t>
+  </si>
+  <si>
+    <t>MSBuild</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/visualstudio/msbuild/msbuild?view=vs-2022</t>
+  </si>
+  <si>
+    <t>Dub</t>
+  </si>
+  <si>
+    <t>https://dub.pm/#:~:text=DUB%20is%20the%20D%20language's,compiled%20package%20for%20your%20platform.</t>
+  </si>
+  <si>
+    <t>Leiningen</t>
+  </si>
+  <si>
+    <t>https://leiningen.org/</t>
+  </si>
+  <si>
+    <t>Boot</t>
+  </si>
+  <si>
+    <t>https://docs.spring.io/spring-boot/docs/2.1.9.RELEASE/reference/html/using-boot-build-systems.html</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>https://elixir-lang.org/getting-started/mix-otp/introduction-to-mix.html</t>
+  </si>
+  <si>
+    <t>Nant</t>
+  </si>
+  <si>
+    <t>http://nant.sourceforge.net/</t>
+  </si>
+  <si>
+    <t>FinalBuilder</t>
+  </si>
+  <si>
+    <t>https://www.finalbuilder.com/finalbuilder</t>
+  </si>
+  <si>
+    <t>Psake</t>
+  </si>
+  <si>
+    <t>https://github.com/psake/psake</t>
+  </si>
+  <si>
+    <t>Jam</t>
+  </si>
+  <si>
+    <t>https://swarm.workshop.perforce.com/view/guest/perforce_software/jam/src/Jam.html</t>
+  </si>
+  <si>
+    <t>Waf</t>
+  </si>
+  <si>
+    <t>https://waf.io/</t>
+  </si>
+  <si>
+    <t>sbt</t>
+  </si>
+  <si>
+    <t>https://www.scala-sbt.org/</t>
+  </si>
+  <si>
+    <t>Scons</t>
+  </si>
+  <si>
+    <t>https://scons.org/</t>
+  </si>
+  <si>
+    <t>Visual Build</t>
+  </si>
+  <si>
+    <t>https://www.kinook.com/VisBuildPro/</t>
+  </si>
+  <si>
+    <t>Meson</t>
+  </si>
+  <si>
+    <t>https://mesonbuild.com/</t>
+  </si>
+  <si>
+    <t>Automake</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/software/automake/manual/html_node/GNU-Build-System.html</t>
+  </si>
+  <si>
+    <t>Premake</t>
+  </si>
+  <si>
+    <t>https://premake.github.io/</t>
+  </si>
+  <si>
+    <t>FastBuild</t>
+  </si>
+  <si>
+    <t>https://www.fastbuild.org/docs/home.html</t>
+  </si>
+  <si>
+    <t>Sharpmake</t>
+  </si>
+  <si>
+    <t>https://github.com/ubisoft/Sharpmake</t>
+  </si>
+  <si>
+    <t>Please</t>
+  </si>
+  <si>
+    <t>https://please.build/</t>
+  </si>
+  <si>
+    <t>Mill</t>
+  </si>
+  <si>
+    <t>https://com-lihaoyi.github.io/mill/mill/Intro_to_Mill.html</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>https://www.pantsbuild.org/</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>https://cakebuild.net/</t>
+  </si>
+  <si>
+    <t>Qbs</t>
+  </si>
+  <si>
+    <t>https://doc.qt.io/qbs/index.html</t>
+  </si>
+  <si>
+    <t>Aimake</t>
+  </si>
+  <si>
+    <t>http://nethack4.org/projects/aimake/</t>
+  </si>
+  <si>
+    <t>Xmake</t>
+  </si>
+  <si>
+    <t>https://xmake.io/#/</t>
   </si>
 </sst>
 </file>
@@ -570,15 +801,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E6FD19-3851-B94F-9B70-E58C943A64A1}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J9"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,10 +838,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -618,33 +852,36 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -653,10 +890,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
@@ -665,92 +902,101 @@
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="J5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>11</v>
@@ -759,28 +1005,29 @@
         <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>11</v>
@@ -789,73 +1036,742 @@
         <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="I9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{3C03B2B0-66F9-5244-A856-F2A42E8059D0}"/>
-    <hyperlink ref="J2" r:id="rId2" display="https://dl.acm.org/doi/pdf/10.1145/3497775.3503687" xr:uid="{509FEA21-1DD1-484E-8E70-F34AA1D5FF7D}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{BE6EC0CB-3F30-534B-AE25-22BA5F69B95F}"/>
-    <hyperlink ref="J3" r:id="rId4" display="https://www.cambridge.org/core/services/aop-cambridge-core/content/view/097CE52C750E69BD16B78C318754C7A4/S0956796820000088a.pdf/build-systems-a-la-carte-theory-and-practice.pdf" xr:uid="{78C400E1-86E3-A04A-A634-36CE9CD4CDC9}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{CB20C02D-2915-DD4D-A203-B22744E2FB3B}"/>
-    <hyperlink ref="I5" r:id="rId6" xr:uid="{F49A385A-A8D8-8642-8404-6F2A9F91E297}"/>
-    <hyperlink ref="I6" r:id="rId7" xr:uid="{E1D11EB7-FF94-4748-B8CB-46EFA8F843F3}"/>
-    <hyperlink ref="I7" r:id="rId8" xr:uid="{C06DBDB6-8C5F-5F47-B703-C18B6B5D16B4}"/>
-    <hyperlink ref="I8" r:id="rId9" xr:uid="{4CDA1698-4B66-F94D-AC73-479B11FF4979}"/>
-    <hyperlink ref="I9" r:id="rId10" xr:uid="{7F7E342E-8E46-8B4C-9390-4225715D5F05}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{2BC34D71-DC91-224F-AF1D-71E31AEF9047}"/>
+    <hyperlink ref="K2" r:id="rId2" display="https://dl.acm.org/doi/pdf/10.1145/3497775.3503687" xr:uid="{6ED7C308-5AB2-AE44-888D-431588F83F1A}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{F25F7188-0FE3-CE4C-BAD5-CCB3EA8F6352}"/>
+    <hyperlink ref="K3" r:id="rId4" display="https://www.cambridge.org/core/services/aop-cambridge-core/content/view/097CE52C750E69BD16B78C318754C7A4/S0956796820000088a.pdf/build-systems-a-la-carte-theory-and-practice.pdf" xr:uid="{4F127A62-EF9A-B340-A297-4D52A11562DA}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{306C02A7-CCF0-3C45-989C-26AE62FFAFE8}"/>
+    <hyperlink ref="I5" r:id="rId6" xr:uid="{B8D28705-0B6E-E941-A0C3-55CD13A99225}"/>
+    <hyperlink ref="I6" r:id="rId7" xr:uid="{2256E85F-B4A7-804F-AE65-1C419AE30FEF}"/>
+    <hyperlink ref="I7" r:id="rId8" xr:uid="{017B6E65-C5DF-AB49-8F20-55F815F4825B}"/>
+    <hyperlink ref="I8" r:id="rId9" xr:uid="{765098AC-EF9B-0A4D-8165-78CEA7AFD048}"/>
+    <hyperlink ref="I9" r:id="rId10" xr:uid="{9CB22F99-D60D-E248-A1ED-D3042A2A6186}"/>
+    <hyperlink ref="I10" r:id="rId11" xr:uid="{3E641FC7-B85F-B841-9461-98D2ED7E8000}"/>
+    <hyperlink ref="I11" r:id="rId12" xr:uid="{0889DB63-8459-C140-9319-FB3C6F0BC06C}"/>
+    <hyperlink ref="I12" r:id="rId13" xr:uid="{9BFC21F7-10A6-D449-80A8-47A6F0A7C6A8}"/>
+    <hyperlink ref="I13" r:id="rId14" xr:uid="{A35FB8D7-13B4-0B4C-B75F-4E2E4184375A}"/>
+    <hyperlink ref="I14" r:id="rId15" xr:uid="{03802008-2F9E-9E4B-8C52-CC83BFFC0F2D}"/>
+    <hyperlink ref="I15" r:id="rId16" xr:uid="{47FAA50F-CA18-D741-A8D9-50616266CE44}"/>
+    <hyperlink ref="I16" r:id="rId17" xr:uid="{FF561629-B5F6-5149-9125-73CE669C77B8}"/>
+    <hyperlink ref="I17" r:id="rId18" xr:uid="{EC7A09AC-57E4-D44F-9DB8-B04F2F8CBF87}"/>
+    <hyperlink ref="I18" r:id="rId19" xr:uid="{6C0B3144-2D5A-424D-A13C-C7C77D4137FF}"/>
+    <hyperlink ref="I19" r:id="rId20" xr:uid="{0606F6E6-319D-1541-A3D1-CC792A1A12F8}"/>
+    <hyperlink ref="I20" r:id="rId21" xr:uid="{2F1CA38F-F2D8-4545-95B8-72BC94D45442}"/>
+    <hyperlink ref="I21" r:id="rId22" xr:uid="{111D2F3F-2387-054F-A18E-86E364086539}"/>
+    <hyperlink ref="I22" r:id="rId23" location=":~:text=DUB%20is%20the%20D%20language's,compiled%20package%20for%20your%20platform." display="https://dub.pm/ - :~:text=DUB%20is%20the%20D%20language's,compiled%20package%20for%20your%20platform." xr:uid="{0ABB8A6B-DDCD-E74D-88DE-D6CAF947EBDD}"/>
+    <hyperlink ref="I23" r:id="rId24" xr:uid="{D0200065-E332-734D-BC3A-3ACEF9EAF43B}"/>
+    <hyperlink ref="I24" r:id="rId25" xr:uid="{B00F7C47-D740-7349-86E2-D1F616F02C0F}"/>
+    <hyperlink ref="I25" r:id="rId26" xr:uid="{207B4AE3-8217-4F43-B370-00DBA2754851}"/>
+    <hyperlink ref="I26" r:id="rId27" xr:uid="{37B93E08-577E-7D48-A6AE-844DF29A09CC}"/>
+    <hyperlink ref="I27" r:id="rId28" xr:uid="{66F980D6-745D-1A4A-AE0A-7CF6E1AB7BCD}"/>
+    <hyperlink ref="I28" r:id="rId29" xr:uid="{B086FE44-F6DE-484F-8D44-CB1B98684B29}"/>
+    <hyperlink ref="I29" r:id="rId30" xr:uid="{B06A0434-DA73-204A-8587-49B0733C2CD4}"/>
+    <hyperlink ref="I30" r:id="rId31" xr:uid="{C013C43F-8530-654B-9D45-B3F2B80209CC}"/>
+    <hyperlink ref="I31" r:id="rId32" xr:uid="{729B28E8-CAC9-A24C-8305-559FC40B94E4}"/>
+    <hyperlink ref="I32" r:id="rId33" xr:uid="{CBC076CF-A6FB-7B4D-A459-C57C77E8744E}"/>
+    <hyperlink ref="I33" r:id="rId34" xr:uid="{93BE8D42-2CC4-6D43-9BF1-8DE4F24A03E1}"/>
+    <hyperlink ref="I34" r:id="rId35" xr:uid="{3B4E15B6-99D8-8245-BA4B-EF1407F2D4CA}"/>
+    <hyperlink ref="I35" r:id="rId36" xr:uid="{2759A5E6-E927-DC41-AFFD-2A8068C23A85}"/>
+    <hyperlink ref="I36" r:id="rId37" xr:uid="{6C5FA7D3-5C81-FB45-9BEE-F5EFC5D8C364}"/>
+    <hyperlink ref="I37" r:id="rId38" xr:uid="{F9CCE41D-4F98-C248-A880-048B9870371C}"/>
+    <hyperlink ref="I38" r:id="rId39" xr:uid="{204C0A5E-E20F-1A4D-B350-510580B371AB}"/>
+    <hyperlink ref="I39" r:id="rId40" xr:uid="{83118512-43A1-0B46-BF72-1697229644D9}"/>
+    <hyperlink ref="I40" r:id="rId41" xr:uid="{DCCDEAC7-4D50-AD47-B2DB-07FAFC231519}"/>
+    <hyperlink ref="I41" r:id="rId42" xr:uid="{061F3AAC-9657-E246-82D1-95FB410CB7A4}"/>
+    <hyperlink ref="I42" r:id="rId43" xr:uid="{FAA2CC7F-1ABD-B841-B0F5-607134BBD9ED}"/>
+    <hyperlink ref="I43" r:id="rId44" xr:uid="{54AF8B6A-40F9-134D-97AD-8437C3EB9F4B}"/>
+    <hyperlink ref="I44" r:id="rId45" xr:uid="{04E04DB1-AD00-BA40-BA32-10F1C8B61FF1}"/>
+    <hyperlink ref="I45" r:id="rId46" location="/" display="https://xmake.io/ - /" xr:uid="{0A4C0B14-2047-C545-91F2-346B573BD76B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>